<commit_message>
309. Best Time to Buy and Sell Stock with Cooldown
309. Best Time to Buy and Sell Stock with Cooldown
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Stocks/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Stocks/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462F1F9-8865-439F-8B2E-6BF964BB81E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4957B2-AF2F-476A-8F49-295596BACF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Question No</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Recurssion,Memoization,Tabulation,Space optimization</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock III</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock IV</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock with cool down period of 1 day</t>
+  </si>
+  <si>
+    <t>Recurssion,Memoization,Tabulation,buy for loop removed</t>
   </si>
 </sst>
 </file>
@@ -99,18 +111,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -163,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -182,21 +188,20 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +485,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,79 +499,110 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>121</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="3" spans="1:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>122</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+    <row r="4" spans="1:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>123</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>188</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>309</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -601,7 +637,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>

</xml_diff>